<commit_message>
update analyses for study 2
</commit_message>
<xml_diff>
--- a/Study 2/Experiment/attentional_competition_task/positions_test_new.xlsx
+++ b/Study 2/Experiment/attentional_competition_task/positions_test_new.xlsx
@@ -5,20 +5,31 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sag22id\Documents\Projects\GCA\gca_avoidance\attentional_competition_task\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sag22id\Documents\Projects\GCA\gca_avoidance\Study 2\Experiment\attentional_competition_task\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{784581A5-F42E-4F2C-9D1C-F0A670BF1415}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0476DB13-51C3-4690-B0A3-08B18AA4779B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12600" yWindow="0" windowWidth="12600" windowHeight="15150" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-38510" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
+    <sheet name="Tabelle1" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -435,19 +446,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56A92758-8D3F-499C-8BA5-36B4DFC0430C}">
   <dimension ref="A1:H121"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -473,7 +484,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -499,7 +510,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -525,7 +536,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -551,7 +562,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -577,7 +588,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>1</v>
       </c>
@@ -603,7 +614,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>1</v>
       </c>
@@ -629,7 +640,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>1</v>
       </c>
@@ -655,7 +666,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>1</v>
       </c>
@@ -681,7 +692,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>1</v>
       </c>
@@ -707,7 +718,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>1</v>
       </c>
@@ -733,7 +744,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>1</v>
       </c>
@@ -759,7 +770,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>1</v>
       </c>
@@ -785,7 +796,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>1</v>
       </c>
@@ -811,7 +822,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>1</v>
       </c>
@@ -837,7 +848,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>1</v>
       </c>
@@ -863,7 +874,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>1</v>
       </c>
@@ -889,7 +900,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>1</v>
       </c>
@@ -915,7 +926,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>1</v>
       </c>
@@ -941,7 +952,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>1</v>
       </c>
@@ -967,7 +978,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>1</v>
       </c>
@@ -993,7 +1004,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>1</v>
       </c>
@@ -1019,7 +1030,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>1</v>
       </c>
@@ -1045,7 +1056,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>1</v>
       </c>
@@ -1071,7 +1082,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>1</v>
       </c>
@@ -1097,7 +1108,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>1</v>
       </c>
@@ -1123,7 +1134,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>1</v>
       </c>
@@ -1149,7 +1160,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>1</v>
       </c>
@@ -1175,7 +1186,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>1</v>
       </c>
@@ -1201,7 +1212,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>1</v>
       </c>
@@ -1227,7 +1238,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>1</v>
       </c>
@@ -1253,7 +1264,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>1</v>
       </c>
@@ -1279,7 +1290,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>1</v>
       </c>
@@ -1305,7 +1316,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>1</v>
       </c>
@@ -1331,7 +1342,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>1</v>
       </c>
@@ -1357,7 +1368,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>1</v>
       </c>
@@ -1383,7 +1394,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>1</v>
       </c>
@@ -1409,7 +1420,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>1</v>
       </c>
@@ -1435,7 +1446,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>1</v>
       </c>
@@ -1461,7 +1472,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>1</v>
       </c>
@@ -1487,7 +1498,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>1</v>
       </c>
@@ -1513,7 +1524,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>1</v>
       </c>
@@ -1539,7 +1550,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>1</v>
       </c>
@@ -1565,7 +1576,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>1</v>
       </c>
@@ -1591,7 +1602,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>1</v>
       </c>
@@ -1617,7 +1628,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>1</v>
       </c>
@@ -1643,7 +1654,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>1</v>
       </c>
@@ -1669,7 +1680,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>1</v>
       </c>
@@ -1695,7 +1706,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>1</v>
       </c>
@@ -1721,7 +1732,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>1</v>
       </c>
@@ -1747,7 +1758,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>1</v>
       </c>
@@ -1773,7 +1784,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>1</v>
       </c>
@@ -1799,7 +1810,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>1</v>
       </c>
@@ -1825,7 +1836,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>1</v>
       </c>
@@ -1851,7 +1862,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>1</v>
       </c>
@@ -1877,7 +1888,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>1</v>
       </c>
@@ -1903,7 +1914,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>1</v>
       </c>
@@ -1929,7 +1940,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>1</v>
       </c>
@@ -1955,7 +1966,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>1</v>
       </c>
@@ -1981,7 +1992,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>1</v>
       </c>
@@ -2007,7 +2018,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>1</v>
       </c>
@@ -2033,7 +2044,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>1</v>
       </c>
@@ -2059,7 +2070,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>1</v>
       </c>
@@ -2085,7 +2096,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>1</v>
       </c>
@@ -2111,7 +2122,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>1</v>
       </c>
@@ -2137,7 +2148,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>1</v>
       </c>
@@ -2163,7 +2174,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
         <v>1</v>
       </c>
@@ -2189,7 +2200,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>1</v>
       </c>
@@ -2215,7 +2226,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
         <v>1</v>
       </c>
@@ -2241,7 +2252,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
         <v>1</v>
       </c>
@@ -2267,7 +2278,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
         <v>1</v>
       </c>
@@ -2293,7 +2304,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
         <v>1</v>
       </c>
@@ -2319,7 +2330,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
         <v>1</v>
       </c>
@@ -2345,7 +2356,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
         <v>1</v>
       </c>
@@ -2371,7 +2382,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
         <v>1</v>
       </c>
@@ -2397,7 +2408,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
         <v>1</v>
       </c>
@@ -2423,7 +2434,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
         <v>1</v>
       </c>
@@ -2449,7 +2460,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
         <v>1</v>
       </c>
@@ -2475,7 +2486,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
         <v>1</v>
       </c>
@@ -2501,7 +2512,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
         <v>1</v>
       </c>
@@ -2527,7 +2538,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
         <v>1</v>
       </c>
@@ -2553,7 +2564,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
         <v>1</v>
       </c>
@@ -2579,7 +2590,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
         <v>1</v>
       </c>
@@ -2605,7 +2616,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
         <v>1</v>
       </c>
@@ -2631,7 +2642,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
         <v>1</v>
       </c>
@@ -2657,7 +2668,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
         <v>1</v>
       </c>
@@ -2683,7 +2694,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
         <v>1</v>
       </c>
@@ -2709,7 +2720,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
         <v>1</v>
       </c>
@@ -2735,7 +2746,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
         <v>1</v>
       </c>
@@ -2761,7 +2772,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
         <v>1</v>
       </c>
@@ -2787,7 +2798,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
         <v>1</v>
       </c>
@@ -2813,7 +2824,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
         <v>1</v>
       </c>
@@ -2839,7 +2850,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
         <v>1</v>
       </c>
@@ -2865,7 +2876,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
         <v>1</v>
       </c>
@@ -2891,7 +2902,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
         <v>1</v>
       </c>
@@ -2917,7 +2928,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
         <v>1</v>
       </c>
@@ -2943,7 +2954,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
         <v>1</v>
       </c>
@@ -2969,7 +2980,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
         <v>1</v>
       </c>
@@ -2995,7 +3006,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
         <v>1</v>
       </c>
@@ -3021,7 +3032,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
         <v>1</v>
       </c>
@@ -3047,7 +3058,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
         <v>1</v>
       </c>
@@ -3073,7 +3084,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
         <v>1</v>
       </c>
@@ -3099,7 +3110,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
         <v>1</v>
       </c>
@@ -3125,7 +3136,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
         <v>1</v>
       </c>
@@ -3151,7 +3162,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
         <v>1</v>
       </c>
@@ -3177,7 +3188,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
         <v>1</v>
       </c>
@@ -3203,7 +3214,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
         <v>1</v>
       </c>
@@ -3229,7 +3240,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="108" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
         <v>1</v>
       </c>
@@ -3255,7 +3266,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="109" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
         <v>1</v>
       </c>
@@ -3281,7 +3292,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="110" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
         <v>1</v>
       </c>
@@ -3307,7 +3318,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="111" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
         <v>1</v>
       </c>
@@ -3333,7 +3344,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="112" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
         <v>1</v>
       </c>
@@ -3359,7 +3370,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="113" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
         <v>1</v>
       </c>
@@ -3385,7 +3396,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="114" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A114" t="s">
         <v>1</v>
       </c>
@@ -3411,7 +3422,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="115" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A115" t="s">
         <v>1</v>
       </c>
@@ -3437,7 +3448,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="116" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A116" t="s">
         <v>1</v>
       </c>
@@ -3463,7 +3474,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="117" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A117" t="s">
         <v>1</v>
       </c>
@@ -3489,7 +3500,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="118" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A118" t="s">
         <v>1</v>
       </c>
@@ -3515,7 +3526,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="119" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A119" t="s">
         <v>1</v>
       </c>
@@ -3541,7 +3552,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="120" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A120" t="s">
         <v>1</v>
       </c>
@@ -3567,7 +3578,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="121" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A121" t="s">
         <v>1</v>
       </c>

</xml_diff>